<commit_message>
1. merged data 2. archived unused data
</commit_message>
<xml_diff>
--- a/sec_apprch/DATA/more/hospital_bed.xlsx
+++ b/sec_apprch/DATA/more/hospital_bed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chen_yenru/Documents/GitHub/Data_Analysis/air_qu/sec_apprch/DATA/more/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47230BBA-64F8-5745-AC2A-559392E83973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F53186-4E5C-AD42-B5CC-C0DE0B62DC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="500" windowWidth="27420" windowHeight="16940" xr2:uid="{083F3BF7-5D64-264A-B0D6-F7FC369A1A68}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="CS2701A1Ac" localSheetId="0">Sheet1!$A$1:$Y$173</definedName>
+    <definedName name="CS2701A1Ac" localSheetId="0">Sheet1!$A$1:$T$173</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -75,13 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t xml:space="preserve"> 總計</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 臺灣地區</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve"> 新北市</t>
   </si>
@@ -131,9 +125,6 @@
     <t xml:space="preserve"> 花蓮縣</t>
   </si>
   <si>
-    <t xml:space="preserve"> 澎湖縣</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 基隆市</t>
   </si>
   <si>
@@ -141,12 +132,6 @@
   </si>
   <si>
     <t xml:space="preserve"> 嘉義市</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 金門縣</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 連江縣</t>
   </si>
   <si>
     <t>year</t>
@@ -505,23 +490,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88031090-2402-2F42-B3E7-455C282D8B35}">
-  <dimension ref="A1:Y24"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="25" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="20" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -580,1791 +563,1431 @@
       <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1998</v>
       </c>
       <c r="B2">
-        <v>56.8</v>
+        <v>28.98</v>
       </c>
       <c r="C2">
-        <v>56.83</v>
+        <v>81.41</v>
       </c>
       <c r="D2">
-        <v>28.98</v>
+        <v>66.14</v>
       </c>
       <c r="E2">
-        <v>81.41</v>
+        <v>52.44</v>
       </c>
       <c r="F2">
-        <v>66.14</v>
+        <v>53.09</v>
       </c>
       <c r="G2">
-        <v>52.44</v>
+        <v>61.33</v>
       </c>
       <c r="H2">
-        <v>53.09</v>
+        <v>87.99</v>
       </c>
       <c r="I2">
-        <v>61.33</v>
+        <v>40.700000000000003</v>
       </c>
       <c r="J2">
-        <v>87.99</v>
+        <v>53.35</v>
       </c>
       <c r="K2">
-        <v>40.700000000000003</v>
+        <v>40.67</v>
       </c>
       <c r="L2">
-        <v>53.35</v>
+        <v>58.68</v>
       </c>
       <c r="M2">
-        <v>40.67</v>
+        <v>28.09</v>
       </c>
       <c r="N2">
-        <v>58.68</v>
+        <v>26.2</v>
       </c>
       <c r="O2">
-        <v>28.09</v>
+        <v>54.12</v>
       </c>
       <c r="P2">
-        <v>26.2</v>
+        <v>51.05</v>
       </c>
       <c r="Q2">
-        <v>54.12</v>
+        <v>226.67</v>
       </c>
       <c r="R2">
-        <v>51.05</v>
+        <v>58.39</v>
       </c>
       <c r="S2">
-        <v>226.67</v>
+        <v>58.02</v>
       </c>
       <c r="T2">
-        <v>53.43</v>
-      </c>
-      <c r="U2">
-        <v>58.39</v>
-      </c>
-      <c r="V2">
-        <v>58.02</v>
-      </c>
-      <c r="W2">
         <v>121.99</v>
       </c>
-      <c r="X2">
-        <v>45.63</v>
-      </c>
-      <c r="Y2">
-        <v>55.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1999</v>
       </c>
       <c r="B3">
-        <v>55.65</v>
+        <v>29.39</v>
       </c>
       <c r="C3">
-        <v>55.69</v>
+        <v>79.28</v>
       </c>
       <c r="D3">
-        <v>29.39</v>
+        <v>66.83</v>
       </c>
       <c r="E3">
-        <v>79.28</v>
+        <v>56.24</v>
       </c>
       <c r="F3">
-        <v>66.83</v>
+        <v>54.44</v>
       </c>
       <c r="G3">
-        <v>56.24</v>
+        <v>60</v>
       </c>
       <c r="H3">
-        <v>54.44</v>
+        <v>80.62</v>
       </c>
       <c r="I3">
-        <v>60</v>
+        <v>43.39</v>
       </c>
       <c r="J3">
-        <v>80.62</v>
+        <v>56</v>
       </c>
       <c r="K3">
-        <v>43.39</v>
+        <v>40.33</v>
       </c>
       <c r="L3">
-        <v>56</v>
+        <v>51.49</v>
       </c>
       <c r="M3">
-        <v>40.33</v>
+        <v>31.61</v>
       </c>
       <c r="N3">
-        <v>51.49</v>
+        <v>31.71</v>
       </c>
       <c r="O3">
-        <v>31.61</v>
+        <v>63.02</v>
       </c>
       <c r="P3">
-        <v>31.71</v>
+        <v>51.29</v>
       </c>
       <c r="Q3">
-        <v>63.02</v>
+        <v>126.83</v>
       </c>
       <c r="R3">
-        <v>51.29</v>
+        <v>57.4</v>
       </c>
       <c r="S3">
-        <v>126.83</v>
+        <v>54.32</v>
       </c>
       <c r="T3">
-        <v>52.01</v>
-      </c>
-      <c r="U3">
-        <v>57.4</v>
-      </c>
-      <c r="V3">
-        <v>54.32</v>
-      </c>
-      <c r="W3">
         <v>120.14</v>
       </c>
-      <c r="X3">
-        <v>39.24</v>
-      </c>
-      <c r="Y3">
-        <v>47.26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2000</v>
       </c>
       <c r="B4">
-        <v>56.78</v>
+        <v>26.44</v>
       </c>
       <c r="C4">
-        <v>56.81</v>
+        <v>79.709999999999994</v>
       </c>
       <c r="D4">
-        <v>26.44</v>
+        <v>68.260000000000005</v>
       </c>
       <c r="E4">
-        <v>79.709999999999994</v>
+        <v>58.32</v>
       </c>
       <c r="F4">
-        <v>68.260000000000005</v>
+        <v>56.04</v>
       </c>
       <c r="G4">
-        <v>58.32</v>
+        <v>61.08</v>
       </c>
       <c r="H4">
-        <v>56.04</v>
+        <v>86.78</v>
       </c>
       <c r="I4">
-        <v>61.08</v>
+        <v>43.07</v>
       </c>
       <c r="J4">
-        <v>86.78</v>
+        <v>61.01</v>
       </c>
       <c r="K4">
-        <v>43.07</v>
+        <v>42.46</v>
       </c>
       <c r="L4">
-        <v>61.01</v>
+        <v>64.67</v>
       </c>
       <c r="M4">
-        <v>42.46</v>
+        <v>34.840000000000003</v>
       </c>
       <c r="N4">
-        <v>64.67</v>
+        <v>46.68</v>
       </c>
       <c r="O4">
-        <v>34.840000000000003</v>
+        <v>60.14</v>
       </c>
       <c r="P4">
-        <v>46.68</v>
+        <v>52.46</v>
       </c>
       <c r="Q4">
-        <v>60.14</v>
+        <v>119.67</v>
       </c>
       <c r="R4">
-        <v>52.46</v>
+        <v>54.99</v>
       </c>
       <c r="S4">
-        <v>119.67</v>
+        <v>49.7</v>
       </c>
       <c r="T4">
-        <v>51.73</v>
-      </c>
-      <c r="U4">
-        <v>54.99</v>
-      </c>
-      <c r="V4">
-        <v>49.7</v>
-      </c>
-      <c r="W4">
         <v>131.94</v>
       </c>
-      <c r="X4">
-        <v>38.270000000000003</v>
-      </c>
-      <c r="Y4">
-        <v>74.260000000000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2001</v>
       </c>
       <c r="B5">
-        <v>56.98</v>
+        <v>26.98</v>
       </c>
       <c r="C5">
-        <v>57.01</v>
+        <v>80.95</v>
       </c>
       <c r="D5">
-        <v>26.98</v>
+        <v>69.48</v>
       </c>
       <c r="E5">
-        <v>80.95</v>
+        <v>61.14</v>
       </c>
       <c r="F5">
-        <v>69.48</v>
+        <v>56.05</v>
       </c>
       <c r="G5">
-        <v>61.14</v>
+        <v>60.94</v>
       </c>
       <c r="H5">
-        <v>56.05</v>
+        <v>81.84</v>
       </c>
       <c r="I5">
-        <v>60.94</v>
+        <v>41.97</v>
       </c>
       <c r="J5">
-        <v>81.84</v>
+        <v>55.51</v>
       </c>
       <c r="K5">
-        <v>41.97</v>
+        <v>41.42</v>
       </c>
       <c r="L5">
-        <v>55.51</v>
+        <v>51.77</v>
       </c>
       <c r="M5">
-        <v>41.42</v>
+        <v>37.33</v>
       </c>
       <c r="N5">
-        <v>51.77</v>
+        <v>49.65</v>
       </c>
       <c r="O5">
-        <v>37.33</v>
+        <v>60.17</v>
       </c>
       <c r="P5">
-        <v>49.65</v>
+        <v>53.72</v>
       </c>
       <c r="Q5">
-        <v>60.17</v>
+        <v>122.05</v>
       </c>
       <c r="R5">
-        <v>53.72</v>
+        <v>63.89</v>
       </c>
       <c r="S5">
-        <v>122.05</v>
+        <v>49.85</v>
       </c>
       <c r="T5">
-        <v>51.48</v>
-      </c>
-      <c r="U5">
-        <v>63.89</v>
-      </c>
-      <c r="V5">
-        <v>49.85</v>
-      </c>
-      <c r="W5">
         <v>122.91</v>
       </c>
-      <c r="X5">
-        <v>44.24</v>
-      </c>
-      <c r="Y5">
-        <v>75.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2002</v>
       </c>
       <c r="B6">
-        <v>59.23</v>
+        <v>27.7</v>
       </c>
       <c r="C6">
-        <v>59.27</v>
+        <v>83.58</v>
       </c>
       <c r="D6">
-        <v>27.7</v>
+        <v>69.91</v>
       </c>
       <c r="E6">
-        <v>83.58</v>
+        <v>64.25</v>
       </c>
       <c r="F6">
-        <v>69.91</v>
+        <v>56.17</v>
       </c>
       <c r="G6">
-        <v>64.25</v>
+        <v>63.76</v>
       </c>
       <c r="H6">
-        <v>56.17</v>
+        <v>84.44</v>
       </c>
       <c r="I6">
-        <v>63.76</v>
+        <v>43.23</v>
       </c>
       <c r="J6">
-        <v>84.44</v>
+        <v>55.73</v>
       </c>
       <c r="K6">
-        <v>43.23</v>
+        <v>42.08</v>
       </c>
       <c r="L6">
-        <v>55.73</v>
+        <v>53.21</v>
       </c>
       <c r="M6">
-        <v>42.08</v>
+        <v>41.67</v>
       </c>
       <c r="N6">
-        <v>53.21</v>
+        <v>58.39</v>
       </c>
       <c r="O6">
-        <v>41.67</v>
+        <v>65.12</v>
       </c>
       <c r="P6">
-        <v>58.39</v>
+        <v>53.7</v>
       </c>
       <c r="Q6">
-        <v>65.12</v>
+        <v>125.63</v>
       </c>
       <c r="R6">
-        <v>53.7</v>
+        <v>65.37</v>
       </c>
       <c r="S6">
-        <v>125.63</v>
+        <v>64.52</v>
       </c>
       <c r="T6">
-        <v>50.62</v>
-      </c>
-      <c r="U6">
-        <v>65.37</v>
-      </c>
-      <c r="V6">
-        <v>64.52</v>
-      </c>
-      <c r="W6">
         <v>128.96</v>
       </c>
-      <c r="X6">
-        <v>43.44</v>
-      </c>
-      <c r="Y6">
-        <v>78.739999999999995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2003</v>
       </c>
       <c r="B7">
-        <v>60.31</v>
+        <v>27.77</v>
       </c>
       <c r="C7">
-        <v>60.35</v>
+        <v>84.99</v>
       </c>
       <c r="D7">
-        <v>27.77</v>
+        <v>70.91</v>
       </c>
       <c r="E7">
-        <v>84.99</v>
+        <v>66.58</v>
       </c>
       <c r="F7">
-        <v>70.91</v>
+        <v>58.21</v>
       </c>
       <c r="G7">
-        <v>66.58</v>
+        <v>66.489999999999995</v>
       </c>
       <c r="H7">
-        <v>58.21</v>
+        <v>86.45</v>
       </c>
       <c r="I7">
-        <v>66.489999999999995</v>
+        <v>45.51</v>
       </c>
       <c r="J7">
-        <v>86.45</v>
+        <v>54.43</v>
       </c>
       <c r="K7">
-        <v>45.51</v>
+        <v>44.12</v>
       </c>
       <c r="L7">
-        <v>54.43</v>
+        <v>53.41</v>
       </c>
       <c r="M7">
-        <v>44.12</v>
+        <v>39.61</v>
       </c>
       <c r="N7">
-        <v>53.41</v>
+        <v>60.72</v>
       </c>
       <c r="O7">
-        <v>39.61</v>
+        <v>62.38</v>
       </c>
       <c r="P7">
-        <v>60.72</v>
+        <v>58.93</v>
       </c>
       <c r="Q7">
-        <v>62.38</v>
+        <v>121.6</v>
       </c>
       <c r="R7">
-        <v>58.93</v>
+        <v>65.44</v>
       </c>
       <c r="S7">
-        <v>121.6</v>
+        <v>65.89</v>
       </c>
       <c r="T7">
-        <v>52.14</v>
-      </c>
-      <c r="U7">
-        <v>65.44</v>
-      </c>
-      <c r="V7">
-        <v>65.89</v>
-      </c>
-      <c r="W7">
         <v>131.19999999999999</v>
       </c>
-      <c r="X7">
-        <v>43.62</v>
-      </c>
-      <c r="Y7">
-        <v>78.36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2004</v>
       </c>
       <c r="B8">
-        <v>63.18</v>
+        <v>29.43</v>
       </c>
       <c r="C8">
-        <v>63.24</v>
+        <v>86.42</v>
       </c>
       <c r="D8">
-        <v>29.43</v>
+        <v>75.45</v>
       </c>
       <c r="E8">
-        <v>86.42</v>
+        <v>69.33</v>
       </c>
       <c r="F8">
-        <v>75.45</v>
+        <v>62.71</v>
       </c>
       <c r="G8">
-        <v>69.33</v>
+        <v>72.5</v>
       </c>
       <c r="H8">
-        <v>62.71</v>
+        <v>86.87</v>
       </c>
       <c r="I8">
-        <v>72.5</v>
+        <v>46.55</v>
       </c>
       <c r="J8">
-        <v>86.87</v>
+        <v>57.24</v>
       </c>
       <c r="K8">
-        <v>46.55</v>
+        <v>45.6</v>
       </c>
       <c r="L8">
-        <v>57.24</v>
+        <v>57.93</v>
       </c>
       <c r="M8">
-        <v>45.6</v>
+        <v>41.95</v>
       </c>
       <c r="N8">
-        <v>57.93</v>
+        <v>64.89</v>
       </c>
       <c r="O8">
-        <v>41.95</v>
+        <v>64.52</v>
       </c>
       <c r="P8">
-        <v>64.89</v>
+        <v>57.37</v>
       </c>
       <c r="Q8">
-        <v>64.52</v>
+        <v>132.49</v>
       </c>
       <c r="R8">
-        <v>57.37</v>
+        <v>66.55</v>
       </c>
       <c r="S8">
-        <v>132.49</v>
+        <v>62.82</v>
       </c>
       <c r="T8">
-        <v>54.13</v>
-      </c>
-      <c r="U8">
-        <v>66.55</v>
-      </c>
-      <c r="V8">
-        <v>62.82</v>
-      </c>
-      <c r="W8">
         <v>132.76</v>
       </c>
-      <c r="X8">
-        <v>40.03</v>
-      </c>
-      <c r="Y8">
-        <v>72.66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2005</v>
       </c>
       <c r="B9">
-        <v>64.290000000000006</v>
+        <v>32.68</v>
       </c>
       <c r="C9">
-        <v>64.349999999999994</v>
+        <v>83.48</v>
       </c>
       <c r="D9">
-        <v>32.68</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="E9">
-        <v>83.48</v>
+        <v>70.36</v>
       </c>
       <c r="F9">
-        <v>76.400000000000006</v>
+        <v>64.14</v>
       </c>
       <c r="G9">
-        <v>70.36</v>
+        <v>73.42</v>
       </c>
       <c r="H9">
-        <v>64.14</v>
+        <v>87.85</v>
       </c>
       <c r="I9">
-        <v>73.42</v>
+        <v>47.5</v>
       </c>
       <c r="J9">
-        <v>87.85</v>
+        <v>60.47</v>
       </c>
       <c r="K9">
-        <v>47.5</v>
+        <v>50.78</v>
       </c>
       <c r="L9">
-        <v>60.47</v>
+        <v>58.44</v>
       </c>
       <c r="M9">
-        <v>50.78</v>
+        <v>41.8</v>
       </c>
       <c r="N9">
-        <v>58.44</v>
+        <v>63.7</v>
       </c>
       <c r="O9">
-        <v>41.8</v>
+        <v>67.34</v>
       </c>
       <c r="P9">
-        <v>63.7</v>
+        <v>59.01</v>
       </c>
       <c r="Q9">
-        <v>67.34</v>
+        <v>133.34</v>
       </c>
       <c r="R9">
-        <v>59.01</v>
+        <v>64.819999999999993</v>
       </c>
       <c r="S9">
-        <v>133.34</v>
+        <v>60.51</v>
       </c>
       <c r="T9">
-        <v>57.95</v>
-      </c>
-      <c r="U9">
-        <v>64.819999999999993</v>
-      </c>
-      <c r="V9">
-        <v>60.51</v>
-      </c>
-      <c r="W9">
         <v>135.66</v>
       </c>
-      <c r="X9">
-        <v>48.25</v>
-      </c>
-      <c r="Y9">
-        <v>42.53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2006</v>
       </c>
       <c r="B10">
-        <v>65.12</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="C10">
-        <v>65.209999999999994</v>
+        <v>82.78</v>
       </c>
       <c r="D10">
-        <v>33.799999999999997</v>
+        <v>75.52</v>
       </c>
       <c r="E10">
-        <v>82.78</v>
+        <v>72.56</v>
       </c>
       <c r="F10">
-        <v>75.52</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="G10">
-        <v>72.56</v>
+        <v>73.680000000000007</v>
       </c>
       <c r="H10">
-        <v>64.900000000000006</v>
+        <v>90.44</v>
       </c>
       <c r="I10">
-        <v>73.680000000000007</v>
+        <v>46.44</v>
       </c>
       <c r="J10">
-        <v>90.44</v>
+        <v>59.32</v>
       </c>
       <c r="K10">
-        <v>46.44</v>
+        <v>56.27</v>
       </c>
       <c r="L10">
-        <v>59.32</v>
+        <v>60.31</v>
       </c>
       <c r="M10">
-        <v>56.27</v>
+        <v>43.31</v>
       </c>
       <c r="N10">
-        <v>60.31</v>
+        <v>62.74</v>
       </c>
       <c r="O10">
-        <v>43.31</v>
+        <v>68.28</v>
       </c>
       <c r="P10">
-        <v>62.74</v>
+        <v>60.05</v>
       </c>
       <c r="Q10">
-        <v>68.28</v>
+        <v>131.65</v>
       </c>
       <c r="R10">
-        <v>60.05</v>
+        <v>67.22</v>
       </c>
       <c r="S10">
-        <v>131.65</v>
+        <v>59.81</v>
       </c>
       <c r="T10">
-        <v>58.4</v>
-      </c>
-      <c r="U10">
-        <v>67.22</v>
-      </c>
-      <c r="V10">
-        <v>59.81</v>
-      </c>
-      <c r="W10">
         <v>140.77000000000001</v>
       </c>
-      <c r="X10">
-        <v>39.869999999999997</v>
-      </c>
-      <c r="Y10">
-        <v>44.96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2007</v>
       </c>
       <c r="B11">
-        <v>65.61</v>
+        <v>34.840000000000003</v>
       </c>
       <c r="C11">
-        <v>65.72</v>
+        <v>85.49</v>
       </c>
       <c r="D11">
-        <v>34.840000000000003</v>
+        <v>72.7</v>
       </c>
       <c r="E11">
-        <v>85.49</v>
+        <v>73.39</v>
       </c>
       <c r="F11">
-        <v>72.7</v>
+        <v>65.02</v>
       </c>
       <c r="G11">
-        <v>73.39</v>
+        <v>73.55</v>
       </c>
       <c r="H11">
-        <v>65.02</v>
+        <v>93.61</v>
       </c>
       <c r="I11">
-        <v>73.55</v>
+        <v>45.52</v>
       </c>
       <c r="J11">
-        <v>93.61</v>
+        <v>60.3</v>
       </c>
       <c r="K11">
-        <v>45.52</v>
+        <v>55.49</v>
       </c>
       <c r="L11">
-        <v>60.3</v>
+        <v>61.02</v>
       </c>
       <c r="M11">
-        <v>55.49</v>
+        <v>47.18</v>
       </c>
       <c r="N11">
-        <v>61.02</v>
+        <v>61.59</v>
       </c>
       <c r="O11">
-        <v>47.18</v>
+        <v>67.180000000000007</v>
       </c>
       <c r="P11">
-        <v>61.59</v>
+        <v>63</v>
       </c>
       <c r="Q11">
-        <v>67.180000000000007</v>
+        <v>130.41</v>
       </c>
       <c r="R11">
-        <v>63</v>
+        <v>68.37</v>
       </c>
       <c r="S11">
-        <v>130.41</v>
+        <v>62.83</v>
       </c>
       <c r="T11">
-        <v>58.23</v>
-      </c>
-      <c r="U11">
-        <v>68.37</v>
-      </c>
-      <c r="V11">
-        <v>62.83</v>
-      </c>
-      <c r="W11">
         <v>143.69999999999999</v>
       </c>
-      <c r="X11">
-        <v>36.67</v>
-      </c>
-      <c r="Y11">
-        <v>47.26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2008</v>
       </c>
       <c r="B12">
-        <v>66.37</v>
+        <v>37.47</v>
       </c>
       <c r="C12">
-        <v>66.5</v>
+        <v>88.69</v>
       </c>
       <c r="D12">
-        <v>37.47</v>
+        <v>72.180000000000007</v>
       </c>
       <c r="E12">
-        <v>88.69</v>
+        <v>72.510000000000005</v>
       </c>
       <c r="F12">
-        <v>72.180000000000007</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="G12">
-        <v>72.510000000000005</v>
+        <v>73.22</v>
       </c>
       <c r="H12">
-        <v>64.900000000000006</v>
+        <v>91.95</v>
       </c>
       <c r="I12">
-        <v>73.22</v>
+        <v>45.03</v>
       </c>
       <c r="J12">
-        <v>91.95</v>
+        <v>64.260000000000005</v>
       </c>
       <c r="K12">
-        <v>45.03</v>
+        <v>60.83</v>
       </c>
       <c r="L12">
-        <v>64.260000000000005</v>
+        <v>61.65</v>
       </c>
       <c r="M12">
-        <v>60.83</v>
+        <v>49.08</v>
       </c>
       <c r="N12">
-        <v>61.65</v>
+        <v>52.27</v>
       </c>
       <c r="O12">
-        <v>49.08</v>
+        <v>66.7</v>
       </c>
       <c r="P12">
-        <v>52.27</v>
+        <v>66.510000000000005</v>
       </c>
       <c r="Q12">
-        <v>66.7</v>
+        <v>129.97999999999999</v>
       </c>
       <c r="R12">
-        <v>66.510000000000005</v>
+        <v>68.38</v>
       </c>
       <c r="S12">
-        <v>129.97999999999999</v>
+        <v>59.53</v>
       </c>
       <c r="T12">
-        <v>57.44</v>
-      </c>
-      <c r="U12">
-        <v>68.38</v>
-      </c>
-      <c r="V12">
-        <v>59.53</v>
-      </c>
-      <c r="W12">
         <v>148.25</v>
       </c>
-      <c r="X12">
-        <v>35.71</v>
-      </c>
-      <c r="Y12">
-        <v>36.9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2009</v>
       </c>
       <c r="B13">
-        <v>67.790000000000006</v>
+        <v>40.15</v>
       </c>
       <c r="C13">
-        <v>67.97</v>
+        <v>91.2</v>
       </c>
       <c r="D13">
-        <v>40.15</v>
+        <v>72.510000000000005</v>
       </c>
       <c r="E13">
-        <v>91.2</v>
+        <v>74.17</v>
       </c>
       <c r="F13">
-        <v>72.510000000000005</v>
+        <v>65.459999999999994</v>
       </c>
       <c r="G13">
-        <v>74.17</v>
+        <v>74.41</v>
       </c>
       <c r="H13">
-        <v>65.459999999999994</v>
+        <v>91.44</v>
       </c>
       <c r="I13">
-        <v>74.41</v>
+        <v>46.78</v>
       </c>
       <c r="J13">
-        <v>91.44</v>
+        <v>65.17</v>
       </c>
       <c r="K13">
-        <v>46.78</v>
+        <v>60.19</v>
       </c>
       <c r="L13">
-        <v>65.17</v>
+        <v>62.69</v>
       </c>
       <c r="M13">
-        <v>60.19</v>
+        <v>52.78</v>
       </c>
       <c r="N13">
-        <v>62.69</v>
+        <v>59.89</v>
       </c>
       <c r="O13">
-        <v>52.78</v>
+        <v>68.09</v>
       </c>
       <c r="P13">
-        <v>59.89</v>
+        <v>68</v>
       </c>
       <c r="Q13">
-        <v>68.09</v>
+        <v>130.16</v>
       </c>
       <c r="R13">
-        <v>68</v>
+        <v>68.47</v>
       </c>
       <c r="S13">
-        <v>130.16</v>
+        <v>59.7</v>
       </c>
       <c r="T13">
-        <v>55.09</v>
-      </c>
-      <c r="U13">
-        <v>68.47</v>
-      </c>
-      <c r="V13">
-        <v>59.7</v>
-      </c>
-      <c r="W13">
         <v>147.85</v>
       </c>
-      <c r="X13">
-        <v>27.72</v>
-      </c>
-      <c r="Y13">
-        <v>36.29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2010</v>
       </c>
       <c r="B14">
-        <v>68.61</v>
+        <v>40.97</v>
       </c>
       <c r="C14">
-        <v>68.790000000000006</v>
+        <v>92.49</v>
       </c>
       <c r="D14">
-        <v>40.97</v>
+        <v>73.23</v>
       </c>
       <c r="E14">
-        <v>92.49</v>
+        <v>73.84</v>
       </c>
       <c r="F14">
-        <v>73.23</v>
+        <v>64.56</v>
       </c>
       <c r="G14">
-        <v>73.84</v>
+        <v>75.44</v>
       </c>
       <c r="H14">
-        <v>64.56</v>
+        <v>92.29</v>
       </c>
       <c r="I14">
-        <v>75.44</v>
+        <v>46.49</v>
       </c>
       <c r="J14">
-        <v>92.29</v>
+        <v>65.16</v>
       </c>
       <c r="K14">
-        <v>46.49</v>
+        <v>61.12</v>
       </c>
       <c r="L14">
-        <v>65.16</v>
+        <v>65.41</v>
       </c>
       <c r="M14">
-        <v>61.12</v>
+        <v>56.52</v>
       </c>
       <c r="N14">
-        <v>65.41</v>
+        <v>62.66</v>
       </c>
       <c r="O14">
-        <v>56.52</v>
+        <v>70.17</v>
       </c>
       <c r="P14">
-        <v>62.66</v>
+        <v>69.58</v>
       </c>
       <c r="Q14">
-        <v>70.17</v>
+        <v>134.65</v>
       </c>
       <c r="R14">
-        <v>69.58</v>
+        <v>68.180000000000007</v>
       </c>
       <c r="S14">
-        <v>134.65</v>
+        <v>60.79</v>
       </c>
       <c r="T14">
-        <v>56.13</v>
-      </c>
-      <c r="U14">
-        <v>68.180000000000007</v>
-      </c>
-      <c r="V14">
-        <v>60.79</v>
-      </c>
-      <c r="W14">
         <v>147.29</v>
       </c>
-      <c r="X14">
-        <v>27.63</v>
-      </c>
-      <c r="Y14">
-        <v>49.28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2011</v>
       </c>
       <c r="B15">
-        <v>69.09</v>
+        <v>42</v>
       </c>
       <c r="C15">
-        <v>69.3</v>
+        <v>93.05</v>
       </c>
       <c r="D15">
-        <v>42</v>
+        <v>72.790000000000006</v>
       </c>
       <c r="E15">
-        <v>93.05</v>
+        <v>75.63</v>
       </c>
       <c r="F15">
-        <v>72.790000000000006</v>
+        <v>63.55</v>
       </c>
       <c r="G15">
-        <v>75.63</v>
+        <v>75.56</v>
       </c>
       <c r="H15">
-        <v>63.55</v>
+        <v>94.32</v>
       </c>
       <c r="I15">
-        <v>75.56</v>
+        <v>44.9</v>
       </c>
       <c r="J15">
-        <v>94.32</v>
+        <v>64.73</v>
       </c>
       <c r="K15">
-        <v>44.9</v>
+        <v>61.01</v>
       </c>
       <c r="L15">
-        <v>64.73</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="M15">
-        <v>61.01</v>
+        <v>56.1</v>
       </c>
       <c r="N15">
-        <v>64.959999999999994</v>
+        <v>63.17</v>
       </c>
       <c r="O15">
-        <v>56.1</v>
+        <v>71.510000000000005</v>
       </c>
       <c r="P15">
-        <v>63.17</v>
+        <v>72.099999999999994</v>
       </c>
       <c r="Q15">
-        <v>71.510000000000005</v>
+        <v>135.02000000000001</v>
       </c>
       <c r="R15">
-        <v>72.099999999999994</v>
+        <v>70.540000000000006</v>
       </c>
       <c r="S15">
-        <v>135.02000000000001</v>
+        <v>62.09</v>
       </c>
       <c r="T15">
-        <v>55.58</v>
-      </c>
-      <c r="U15">
-        <v>70.540000000000006</v>
-      </c>
-      <c r="V15">
-        <v>62.09</v>
-      </c>
-      <c r="W15">
         <v>150.66999999999999</v>
       </c>
-      <c r="X15">
-        <v>25.89</v>
-      </c>
-      <c r="Y15">
-        <v>54.42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2012</v>
       </c>
       <c r="B16">
-        <v>69.010000000000005</v>
+        <v>42.21</v>
       </c>
       <c r="C16">
-        <v>69.239999999999995</v>
+        <v>92.84</v>
       </c>
       <c r="D16">
-        <v>42.21</v>
+        <v>72.31</v>
       </c>
       <c r="E16">
-        <v>92.84</v>
+        <v>75.03</v>
       </c>
       <c r="F16">
-        <v>72.31</v>
+        <v>63.53</v>
       </c>
       <c r="G16">
-        <v>75.03</v>
+        <v>75.510000000000005</v>
       </c>
       <c r="H16">
-        <v>63.53</v>
+        <v>93.2</v>
       </c>
       <c r="I16">
-        <v>75.510000000000005</v>
+        <v>44.54</v>
       </c>
       <c r="J16">
-        <v>93.2</v>
+        <v>62.33</v>
       </c>
       <c r="K16">
-        <v>44.54</v>
+        <v>60.37</v>
       </c>
       <c r="L16">
-        <v>62.33</v>
+        <v>65.84</v>
       </c>
       <c r="M16">
-        <v>60.37</v>
+        <v>56.33</v>
       </c>
       <c r="N16">
-        <v>65.84</v>
+        <v>63.12</v>
       </c>
       <c r="O16">
-        <v>56.33</v>
+        <v>73</v>
       </c>
       <c r="P16">
-        <v>63.12</v>
+        <v>73.41</v>
       </c>
       <c r="Q16">
-        <v>73</v>
+        <v>134.31</v>
       </c>
       <c r="R16">
-        <v>73.41</v>
+        <v>74.56</v>
       </c>
       <c r="S16">
-        <v>134.31</v>
+        <v>62.58</v>
       </c>
       <c r="T16">
-        <v>53.72</v>
-      </c>
-      <c r="U16">
-        <v>74.56</v>
-      </c>
-      <c r="V16">
-        <v>62.58</v>
-      </c>
-      <c r="W16">
         <v>153.6</v>
       </c>
-      <c r="X16">
-        <v>23.78</v>
-      </c>
-      <c r="Y16">
-        <v>48.63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2013</v>
       </c>
       <c r="B17">
-        <v>68.209999999999994</v>
+        <v>41.13</v>
       </c>
       <c r="C17">
-        <v>68.459999999999994</v>
+        <v>90.23</v>
       </c>
       <c r="D17">
-        <v>41.13</v>
+        <v>72.349999999999994</v>
       </c>
       <c r="E17">
-        <v>90.23</v>
+        <v>74.75</v>
       </c>
       <c r="F17">
-        <v>72.349999999999994</v>
+        <v>63.84</v>
       </c>
       <c r="G17">
-        <v>74.75</v>
+        <v>74.739999999999995</v>
       </c>
       <c r="H17">
-        <v>63.84</v>
+        <v>91.52</v>
       </c>
       <c r="I17">
-        <v>74.739999999999995</v>
+        <v>43.81</v>
       </c>
       <c r="J17">
-        <v>91.52</v>
+        <v>58.63</v>
       </c>
       <c r="K17">
-        <v>43.81</v>
+        <v>59.87</v>
       </c>
       <c r="L17">
-        <v>58.63</v>
+        <v>64.069999999999993</v>
       </c>
       <c r="M17">
-        <v>59.87</v>
+        <v>56.27</v>
       </c>
       <c r="N17">
-        <v>64.069999999999993</v>
+        <v>65</v>
       </c>
       <c r="O17">
-        <v>56.27</v>
+        <v>71.489999999999995</v>
       </c>
       <c r="P17">
-        <v>65</v>
+        <v>69.61</v>
       </c>
       <c r="Q17">
-        <v>71.489999999999995</v>
+        <v>135.04</v>
       </c>
       <c r="R17">
-        <v>69.61</v>
+        <v>76.739999999999995</v>
       </c>
       <c r="S17">
-        <v>135.04</v>
+        <v>63.97</v>
       </c>
       <c r="T17">
-        <v>54.48</v>
-      </c>
-      <c r="U17">
-        <v>76.739999999999995</v>
-      </c>
-      <c r="V17">
-        <v>63.97</v>
-      </c>
-      <c r="W17">
         <v>152.99</v>
       </c>
-      <c r="X17">
-        <v>22.37</v>
-      </c>
-      <c r="Y17">
-        <v>45.21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2014</v>
       </c>
       <c r="B18">
-        <v>68.91</v>
+        <v>42.85</v>
       </c>
       <c r="C18">
-        <v>69.12</v>
+        <v>92.14</v>
       </c>
       <c r="D18">
-        <v>42.85</v>
+        <v>72.52</v>
       </c>
       <c r="E18">
-        <v>92.14</v>
+        <v>75.84</v>
       </c>
       <c r="F18">
-        <v>72.52</v>
+        <v>65.69</v>
       </c>
       <c r="G18">
-        <v>75.84</v>
+        <v>75.42</v>
       </c>
       <c r="H18">
-        <v>65.69</v>
+        <v>84.75</v>
       </c>
       <c r="I18">
-        <v>75.42</v>
+        <v>43.45</v>
       </c>
       <c r="J18">
-        <v>84.75</v>
+        <v>60.34</v>
       </c>
       <c r="K18">
-        <v>43.45</v>
+        <v>59.6</v>
       </c>
       <c r="L18">
-        <v>60.34</v>
+        <v>64.069999999999993</v>
       </c>
       <c r="M18">
-        <v>59.6</v>
+        <v>56.82</v>
       </c>
       <c r="N18">
-        <v>64.069999999999993</v>
+        <v>64.67</v>
       </c>
       <c r="O18">
-        <v>56.82</v>
+        <v>69.040000000000006</v>
       </c>
       <c r="P18">
-        <v>64.67</v>
+        <v>69.27</v>
       </c>
       <c r="Q18">
-        <v>69.040000000000006</v>
+        <v>134.65</v>
       </c>
       <c r="R18">
-        <v>69.27</v>
+        <v>78.8</v>
       </c>
       <c r="S18">
-        <v>134.65</v>
+        <v>65.599999999999994</v>
       </c>
       <c r="T18">
-        <v>53.75</v>
-      </c>
-      <c r="U18">
-        <v>78.8</v>
-      </c>
-      <c r="V18">
-        <v>65.599999999999994</v>
-      </c>
-      <c r="W18">
         <v>146.59</v>
       </c>
-      <c r="X18">
-        <v>33.04</v>
-      </c>
-      <c r="Y18">
-        <v>43.98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2015</v>
       </c>
       <c r="B19">
-        <v>69.03</v>
+        <v>43.29</v>
       </c>
       <c r="C19">
-        <v>69.28</v>
+        <v>92.59</v>
       </c>
       <c r="D19">
-        <v>43.29</v>
+        <v>70.430000000000007</v>
       </c>
       <c r="E19">
-        <v>92.59</v>
+        <v>76.05</v>
       </c>
       <c r="F19">
-        <v>70.430000000000007</v>
+        <v>67.42</v>
       </c>
       <c r="G19">
-        <v>76.05</v>
+        <v>76.569999999999993</v>
       </c>
       <c r="H19">
-        <v>67.42</v>
+        <v>84.98</v>
       </c>
       <c r="I19">
-        <v>76.569999999999993</v>
+        <v>45.13</v>
       </c>
       <c r="J19">
-        <v>84.98</v>
+        <v>58.89</v>
       </c>
       <c r="K19">
-        <v>45.13</v>
+        <v>59.31</v>
       </c>
       <c r="L19">
-        <v>58.89</v>
+        <v>64.459999999999994</v>
       </c>
       <c r="M19">
-        <v>59.31</v>
+        <v>57.37</v>
       </c>
       <c r="N19">
-        <v>64.459999999999994</v>
+        <v>64.92</v>
       </c>
       <c r="O19">
-        <v>57.37</v>
+        <v>68.53</v>
       </c>
       <c r="P19">
-        <v>64.92</v>
+        <v>67.7</v>
       </c>
       <c r="Q19">
-        <v>68.53</v>
+        <v>131.41</v>
       </c>
       <c r="R19">
-        <v>67.7</v>
+        <v>79.010000000000005</v>
       </c>
       <c r="S19">
-        <v>131.41</v>
+        <v>65.11</v>
       </c>
       <c r="T19">
-        <v>53.57</v>
-      </c>
-      <c r="U19">
-        <v>79.010000000000005</v>
-      </c>
-      <c r="V19">
-        <v>65.11</v>
-      </c>
-      <c r="W19">
         <v>143.84</v>
       </c>
-      <c r="X19">
-        <v>27.86</v>
-      </c>
-      <c r="Y19">
-        <v>41.44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2016</v>
       </c>
       <c r="B20">
-        <v>69.31</v>
+        <v>43.87</v>
       </c>
       <c r="C20">
-        <v>69.56</v>
+        <v>93.02</v>
       </c>
       <c r="D20">
-        <v>43.87</v>
+        <v>69.52</v>
       </c>
       <c r="E20">
-        <v>93.02</v>
+        <v>76.39</v>
       </c>
       <c r="F20">
-        <v>69.52</v>
+        <v>68.08</v>
       </c>
       <c r="G20">
-        <v>76.39</v>
+        <v>77.989999999999995</v>
       </c>
       <c r="H20">
-        <v>68.08</v>
+        <v>85.37</v>
       </c>
       <c r="I20">
-        <v>77.989999999999995</v>
+        <v>44.48</v>
       </c>
       <c r="J20">
-        <v>85.37</v>
+        <v>58.94</v>
       </c>
       <c r="K20">
-        <v>44.48</v>
+        <v>59.28</v>
       </c>
       <c r="L20">
-        <v>58.94</v>
+        <v>64.81</v>
       </c>
       <c r="M20">
-        <v>59.28</v>
+        <v>56.33</v>
       </c>
       <c r="N20">
-        <v>64.81</v>
+        <v>66.23</v>
       </c>
       <c r="O20">
-        <v>56.33</v>
+        <v>67.53</v>
       </c>
       <c r="P20">
-        <v>66.23</v>
+        <v>67.75</v>
       </c>
       <c r="Q20">
-        <v>67.53</v>
+        <v>132.21</v>
       </c>
       <c r="R20">
-        <v>67.75</v>
+        <v>78.42</v>
       </c>
       <c r="S20">
-        <v>132.21</v>
+        <v>64.05</v>
       </c>
       <c r="T20">
-        <v>52.78</v>
-      </c>
-      <c r="U20">
-        <v>78.42</v>
-      </c>
-      <c r="V20">
-        <v>64.05</v>
-      </c>
-      <c r="W20">
         <v>146.11000000000001</v>
       </c>
-      <c r="X20">
-        <v>28.27</v>
-      </c>
-      <c r="Y20">
-        <v>41.29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2017</v>
       </c>
       <c r="B21">
-        <v>69.83</v>
+        <v>45.11</v>
       </c>
       <c r="C21">
-        <v>70.11</v>
+        <v>94.02</v>
       </c>
       <c r="D21">
-        <v>45.11</v>
+        <v>68.8</v>
       </c>
       <c r="E21">
-        <v>94.02</v>
+        <v>77.650000000000006</v>
       </c>
       <c r="F21">
-        <v>68.8</v>
+        <v>68.34</v>
       </c>
       <c r="G21">
-        <v>77.650000000000006</v>
+        <v>78.31</v>
       </c>
       <c r="H21">
-        <v>68.34</v>
+        <v>85.17</v>
       </c>
       <c r="I21">
-        <v>78.31</v>
+        <v>43.56</v>
       </c>
       <c r="J21">
-        <v>85.17</v>
+        <v>61.28</v>
       </c>
       <c r="K21">
-        <v>43.56</v>
+        <v>59.42</v>
       </c>
       <c r="L21">
-        <v>61.28</v>
+        <v>66.62</v>
       </c>
       <c r="M21">
-        <v>59.42</v>
+        <v>56.14</v>
       </c>
       <c r="N21">
-        <v>66.62</v>
+        <v>66.34</v>
       </c>
       <c r="O21">
-        <v>56.14</v>
+        <v>68.2</v>
       </c>
       <c r="P21">
-        <v>66.34</v>
+        <v>69.28</v>
       </c>
       <c r="Q21">
-        <v>68.2</v>
+        <v>131.72999999999999</v>
       </c>
       <c r="R21">
-        <v>69.28</v>
+        <v>77.67</v>
       </c>
       <c r="S21">
-        <v>131.72999999999999</v>
+        <v>62.91</v>
       </c>
       <c r="T21">
-        <v>52.37</v>
-      </c>
-      <c r="U21">
-        <v>77.67</v>
-      </c>
-      <c r="V21">
-        <v>62.91</v>
-      </c>
-      <c r="W21">
         <v>148.91999999999999</v>
       </c>
-      <c r="X21">
-        <v>24.95</v>
-      </c>
-      <c r="Y21">
-        <v>40.369999999999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2018</v>
       </c>
       <c r="B22">
-        <v>71.02</v>
+        <v>46.79</v>
       </c>
       <c r="C22">
-        <v>71.31</v>
+        <v>95.42</v>
       </c>
       <c r="D22">
-        <v>46.79</v>
+        <v>68.41</v>
       </c>
       <c r="E22">
-        <v>95.42</v>
+        <v>78.67</v>
       </c>
       <c r="F22">
-        <v>68.41</v>
+        <v>70.150000000000006</v>
       </c>
       <c r="G22">
-        <v>78.67</v>
+        <v>80.36</v>
       </c>
       <c r="H22">
-        <v>70.150000000000006</v>
+        <v>85.74</v>
       </c>
       <c r="I22">
-        <v>80.36</v>
+        <v>46.07</v>
       </c>
       <c r="J22">
-        <v>85.74</v>
+        <v>60.98</v>
       </c>
       <c r="K22">
-        <v>46.07</v>
+        <v>62.3</v>
       </c>
       <c r="L22">
-        <v>60.98</v>
+        <v>68.209999999999994</v>
       </c>
       <c r="M22">
-        <v>62.3</v>
+        <v>56.72</v>
       </c>
       <c r="N22">
-        <v>68.209999999999994</v>
+        <v>65.89</v>
       </c>
       <c r="O22">
-        <v>56.72</v>
+        <v>68.89</v>
       </c>
       <c r="P22">
-        <v>65.89</v>
+        <v>68.790000000000006</v>
       </c>
       <c r="Q22">
-        <v>68.89</v>
+        <v>133.18</v>
       </c>
       <c r="R22">
-        <v>68.790000000000006</v>
+        <v>78.400000000000006</v>
       </c>
       <c r="S22">
-        <v>133.18</v>
+        <v>63.17</v>
       </c>
       <c r="T22">
-        <v>51.8</v>
-      </c>
-      <c r="U22">
-        <v>78.400000000000006</v>
-      </c>
-      <c r="V22">
-        <v>63.17</v>
-      </c>
-      <c r="W22">
         <v>148.72</v>
       </c>
-      <c r="X22">
-        <v>24.63</v>
-      </c>
-      <c r="Y22">
-        <v>39.83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2019</v>
       </c>
       <c r="B23">
-        <v>71.290000000000006</v>
+        <v>46.98</v>
       </c>
       <c r="C23">
-        <v>71.59</v>
+        <v>95.96</v>
       </c>
       <c r="D23">
-        <v>46.98</v>
+        <v>67.34</v>
       </c>
       <c r="E23">
-        <v>95.96</v>
+        <v>79.67</v>
       </c>
       <c r="F23">
-        <v>67.34</v>
+        <v>70.58</v>
       </c>
       <c r="G23">
-        <v>79.67</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="H23">
-        <v>70.58</v>
+        <v>85.91</v>
       </c>
       <c r="I23">
-        <v>80.900000000000006</v>
+        <v>49.53</v>
       </c>
       <c r="J23">
-        <v>85.91</v>
+        <v>62.11</v>
       </c>
       <c r="K23">
-        <v>49.53</v>
+        <v>62.05</v>
       </c>
       <c r="L23">
-        <v>62.11</v>
+        <v>68.53</v>
       </c>
       <c r="M23">
-        <v>62.05</v>
+        <v>56.76</v>
       </c>
       <c r="N23">
-        <v>68.53</v>
+        <v>66.430000000000007</v>
       </c>
       <c r="O23">
-        <v>56.76</v>
+        <v>70.069999999999993</v>
       </c>
       <c r="P23">
-        <v>66.430000000000007</v>
+        <v>69.38</v>
       </c>
       <c r="Q23">
-        <v>70.069999999999993</v>
+        <v>130.94</v>
       </c>
       <c r="R23">
-        <v>69.38</v>
+        <v>77.69</v>
       </c>
       <c r="S23">
-        <v>130.94</v>
+        <v>63.19</v>
       </c>
       <c r="T23">
-        <v>52.85</v>
-      </c>
-      <c r="U23">
-        <v>77.69</v>
-      </c>
-      <c r="V23">
-        <v>63.19</v>
-      </c>
-      <c r="W23">
         <v>149.05000000000001</v>
       </c>
-      <c r="X23">
-        <v>23.47</v>
-      </c>
-      <c r="Y23">
-        <v>39.729999999999997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2020</v>
       </c>
       <c r="B24">
-        <v>72.06</v>
+        <v>48.38</v>
       </c>
       <c r="C24">
-        <v>72.37</v>
+        <v>98.09</v>
       </c>
       <c r="D24">
-        <v>48.38</v>
+        <v>67.08</v>
       </c>
       <c r="E24">
-        <v>98.09</v>
+        <v>78.62</v>
       </c>
       <c r="F24">
-        <v>67.08</v>
+        <v>70.88</v>
       </c>
       <c r="G24">
-        <v>78.62</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="H24">
-        <v>70.88</v>
+        <v>86.14</v>
       </c>
       <c r="I24">
-        <v>81.599999999999994</v>
+        <v>53.54</v>
       </c>
       <c r="J24">
-        <v>86.14</v>
+        <v>63.23</v>
       </c>
       <c r="K24">
-        <v>53.54</v>
+        <v>63.81</v>
       </c>
       <c r="L24">
-        <v>63.23</v>
+        <v>69.680000000000007</v>
       </c>
       <c r="M24">
-        <v>63.81</v>
+        <v>57.78</v>
       </c>
       <c r="N24">
-        <v>69.680000000000007</v>
+        <v>67.349999999999994</v>
       </c>
       <c r="O24">
-        <v>57.78</v>
+        <v>71.25</v>
       </c>
       <c r="P24">
-        <v>67.349999999999994</v>
+        <v>70.569999999999993</v>
       </c>
       <c r="Q24">
-        <v>71.25</v>
+        <v>133.12</v>
       </c>
       <c r="R24">
-        <v>70.569999999999993</v>
+        <v>79.09</v>
       </c>
       <c r="S24">
-        <v>133.12</v>
+        <v>62.65</v>
       </c>
       <c r="T24">
-        <v>53.8</v>
-      </c>
-      <c r="U24">
-        <v>79.09</v>
-      </c>
-      <c r="V24">
-        <v>62.65</v>
-      </c>
-      <c r="W24">
         <v>150.63999999999999</v>
-      </c>
-      <c r="X24">
-        <v>24.04</v>
-      </c>
-      <c r="Y24">
-        <v>39.159999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>